<commit_message>
After adding testsuite.xml and fluent wait(testcases 1 to 10)
</commit_message>
<xml_diff>
--- a/data/TC10_BookedHotelPrice.xlsx
+++ b/data/TC10_BookedHotelPrice.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>User Name</t>
   </si>
@@ -61,9 +61,6 @@
     <t>2 - Two</t>
   </si>
   <si>
-    <t>21/05/2016</t>
-  </si>
-  <si>
     <t>1 - One</t>
   </si>
   <si>
@@ -115,7 +112,16 @@
     <t>588</t>
   </si>
   <si>
-    <t>22/05/2016</t>
+    <t>price</t>
+  </si>
+  <si>
+    <t>AUD $ 250</t>
+  </si>
+  <si>
+    <t>29/05/2016</t>
+  </si>
+  <si>
+    <t>30/05/2016</t>
   </si>
 </sst>
 </file>
@@ -458,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,7 +491,7 @@
     <col min="17" max="17" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -514,31 +520,34 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>19</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>21</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" t="s">
-        <v>24</v>
+      <c r="R1" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -558,37 +567,40 @@
         <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="J2" t="s">
+        <v>24</v>
+      </c>
+      <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" t="s">
         <v>33</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" t="s">
-        <v>27</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>